<commit_message>
Commit a typo in 2023 exam
</commit_message>
<xml_diff>
--- a/derivatives/homework/exam_solution.xlsx
+++ b/derivatives/homework/exam_solution.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ABak\latex\derivatives\homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DA7A0A-7F94-4B9F-A8C5-4A8944E53DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4F2C7A-E753-46B5-A576-8EAD7C9802B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{CC961C6A-2198-48A3-9945-1D9265B72C7C}"/>
   </bookViews>
@@ -652,12 +652,6 @@
     <t>the risk system, which operates 24x7, was showing Artem that his option</t>
   </si>
   <si>
-    <t>was constantly appreciating and generating profits. What risk unexpectedly</t>
-  </si>
-  <si>
-    <t>helped Artem?</t>
-  </si>
-  <si>
     <t>A. Delta</t>
   </si>
   <si>
@@ -974,6 +968,12 @@
   </si>
   <si>
     <t>corporate bond is $1.</t>
+  </si>
+  <si>
+    <t>was constantly depreciating and generating losses. What risk unexpectedly</t>
+  </si>
+  <si>
+    <t>hurt Artem?</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1047,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1075,7 +1075,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2512,9 +2511,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2552,7 +2551,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2658,7 +2657,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2800,7 +2799,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2808,10 +2807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83242A6E-E45E-4CD4-BA94-7BDA675F44DA}">
-  <dimension ref="A1:L88"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2898,42 +2897,42 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -2941,29 +2940,29 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2973,41 +2972,38 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>178</v>
       </c>
@@ -3016,47 +3012,45 @@
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>186</v>
       </c>
@@ -3147,52 +3141,52 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>203</v>
+        <v>309</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>204</v>
+        <v>310</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -3220,32 +3214,32 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3270,72 +3264,72 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -3492,62 +3486,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -6610,102 +6604,102 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -6983,87 +6977,87 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -7450,7 +7444,7 @@
         <v>88692.043671715743</v>
       </c>
       <c r="D42" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -7948,127 +7942,127 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>